<commit_message>
Added some a script to scrape liquor
</commit_message>
<xml_diff>
--- a/CPI basket.xlsx
+++ b/CPI basket.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive - Kenya National Bureau of Statisitics\CPI\Codes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive\Desktop\Web Scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47172BBD-1869-446D-BA21-670E6454695A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10185"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basket" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Basket!$A$1:$B$331</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1025,7 +1029,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1364,19 +1368,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B331"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="64.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.76953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1384,7 +1389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1392,7 +1397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1400,7 +1405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1408,7 +1413,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1416,7 +1421,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1424,7 +1429,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1432,7 +1437,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1440,7 +1445,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1448,7 +1453,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1456,7 +1461,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1464,7 +1469,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1472,7 +1477,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1480,7 +1485,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1488,7 +1493,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1496,7 +1501,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1504,7 +1509,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1512,7 +1517,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1520,7 +1525,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1528,7 +1533,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1536,7 +1541,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1544,7 +1549,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1552,7 +1557,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1560,7 +1565,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1568,7 +1573,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1576,7 +1581,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1584,7 +1589,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1592,7 +1597,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1600,7 +1605,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1608,7 +1613,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1616,7 +1621,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1624,7 +1629,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1632,7 +1637,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1640,7 +1645,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1648,7 +1653,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1656,7 +1661,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1664,7 +1669,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1672,7 +1677,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1680,7 +1685,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1688,7 +1693,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1696,7 +1701,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1704,7 +1709,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1712,7 +1717,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1720,7 +1725,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1728,7 +1733,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1736,7 +1741,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1744,7 +1749,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1752,7 +1757,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1760,7 +1765,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1768,7 +1773,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -1776,7 +1781,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -1784,7 +1789,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -1792,7 +1797,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -1800,7 +1805,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -1808,7 +1813,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -1816,7 +1821,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -1824,7 +1829,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -1832,7 +1837,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -1840,7 +1845,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -1848,7 +1853,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -1856,7 +1861,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -1864,7 +1869,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -1872,7 +1877,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -1880,7 +1885,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -1888,7 +1893,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -1896,7 +1901,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -1904,7 +1909,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -1912,7 +1917,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -1920,7 +1925,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -1928,7 +1933,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -1936,7 +1941,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -1944,7 +1949,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -1952,7 +1957,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -1960,7 +1965,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -1968,7 +1973,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -1976,7 +1981,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -1984,7 +1989,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -1992,7 +1997,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -2000,7 +2005,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -2008,7 +2013,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -2016,7 +2021,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -2024,7 +2029,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -2032,7 +2037,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -2040,7 +2045,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -2048,7 +2053,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -2056,7 +2061,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -2064,7 +2069,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -2072,7 +2077,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -2080,7 +2085,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -2088,7 +2093,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -2096,7 +2101,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -2104,7 +2109,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -2112,7 +2117,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -2120,7 +2125,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -2128,7 +2133,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -2136,7 +2141,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -2144,7 +2149,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -2152,7 +2157,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -2160,7 +2165,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -2168,7 +2173,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -2176,7 +2181,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -2184,7 +2189,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -2192,7 +2197,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -2200,7 +2205,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -2208,7 +2213,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -2216,7 +2221,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -2224,7 +2229,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -2232,7 +2237,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -2240,7 +2245,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -2248,7 +2253,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A110" s="2">
         <v>109</v>
       </c>
@@ -2256,7 +2261,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -2264,7 +2269,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -2272,7 +2277,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -2280,7 +2285,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -2288,7 +2293,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -2296,7 +2301,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -2304,7 +2309,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -2312,7 +2317,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -2320,7 +2325,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -2328,7 +2333,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A120" s="2">
         <v>119</v>
       </c>
@@ -2336,7 +2341,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -2344,7 +2349,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A122" s="2">
         <v>121</v>
       </c>
@@ -2352,7 +2357,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -2360,7 +2365,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A124" s="2">
         <v>123</v>
       </c>
@@ -2368,7 +2373,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A125" s="2">
         <v>124</v>
       </c>
@@ -2376,7 +2381,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A126" s="2">
         <v>125</v>
       </c>
@@ -2384,7 +2389,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A127" s="2">
         <v>126</v>
       </c>
@@ -2392,7 +2397,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A128" s="2">
         <v>127</v>
       </c>
@@ -2400,7 +2405,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A129" s="2">
         <v>128</v>
       </c>
@@ -2408,7 +2413,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A130" s="2">
         <v>129</v>
       </c>
@@ -2416,7 +2421,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A131" s="2">
         <v>130</v>
       </c>
@@ -2424,7 +2429,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A132" s="2">
         <v>131</v>
       </c>
@@ -2432,7 +2437,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A133" s="2">
         <v>132</v>
       </c>
@@ -2440,7 +2445,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A134" s="2">
         <v>133</v>
       </c>
@@ -2448,7 +2453,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A135" s="2">
         <v>134</v>
       </c>
@@ -2456,7 +2461,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A136" s="2">
         <v>135</v>
       </c>
@@ -2464,7 +2469,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A137" s="2">
         <v>136</v>
       </c>
@@ -2472,7 +2477,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A138" s="2">
         <v>137</v>
       </c>
@@ -2480,7 +2485,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A139" s="2">
         <v>138</v>
       </c>
@@ -2488,7 +2493,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A140" s="2">
         <v>139</v>
       </c>
@@ -2496,7 +2501,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A141" s="2">
         <v>140</v>
       </c>
@@ -2504,7 +2509,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A142" s="2">
         <v>141</v>
       </c>
@@ -2512,7 +2517,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A143" s="2">
         <v>142</v>
       </c>
@@ -2520,7 +2525,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A144" s="2">
         <v>143</v>
       </c>
@@ -2528,7 +2533,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A145" s="2">
         <v>144</v>
       </c>
@@ -2536,7 +2541,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A146" s="2">
         <v>145</v>
       </c>
@@ -2544,7 +2549,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A147" s="2">
         <v>146</v>
       </c>
@@ -2552,7 +2557,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A148" s="2">
         <v>147</v>
       </c>
@@ -2560,7 +2565,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A149" s="2">
         <v>148</v>
       </c>
@@ -2568,7 +2573,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A150" s="2">
         <v>149</v>
       </c>
@@ -2576,7 +2581,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A151" s="2">
         <v>150</v>
       </c>
@@ -2584,7 +2589,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A152" s="2">
         <v>151</v>
       </c>
@@ -2592,7 +2597,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A153" s="2">
         <v>152</v>
       </c>
@@ -2600,7 +2605,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A154" s="2">
         <v>153</v>
       </c>
@@ -2608,7 +2613,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A155" s="2">
         <v>154</v>
       </c>
@@ -2616,7 +2621,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A156" s="2">
         <v>155</v>
       </c>
@@ -2624,7 +2629,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A157" s="2">
         <v>156</v>
       </c>
@@ -2632,7 +2637,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A158" s="2">
         <v>157</v>
       </c>
@@ -2640,7 +2645,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A159" s="2">
         <v>158</v>
       </c>
@@ -2648,7 +2653,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A160" s="2">
         <v>159</v>
       </c>
@@ -2656,7 +2661,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A161" s="2">
         <v>160</v>
       </c>
@@ -2664,7 +2669,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A162" s="2">
         <v>161</v>
       </c>
@@ -2672,7 +2677,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A163" s="2">
         <v>162</v>
       </c>
@@ -2680,7 +2685,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A164" s="2">
         <v>163</v>
       </c>
@@ -2688,7 +2693,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A165" s="2">
         <v>164</v>
       </c>
@@ -2696,7 +2701,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A166" s="2">
         <v>165</v>
       </c>
@@ -2704,7 +2709,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A167" s="2">
         <v>166</v>
       </c>
@@ -2712,7 +2717,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A168" s="2">
         <v>167</v>
       </c>
@@ -2720,7 +2725,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A169" s="2">
         <v>168</v>
       </c>
@@ -2728,7 +2733,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A170" s="2">
         <v>169</v>
       </c>
@@ -2736,7 +2741,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A171" s="2">
         <v>170</v>
       </c>
@@ -2744,7 +2749,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A172" s="2">
         <v>171</v>
       </c>
@@ -2752,7 +2757,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A173" s="2">
         <v>172</v>
       </c>
@@ -2760,7 +2765,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A174" s="2">
         <v>173</v>
       </c>
@@ -2768,7 +2773,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A175" s="2">
         <v>174</v>
       </c>
@@ -2776,7 +2781,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A176" s="2">
         <v>175</v>
       </c>
@@ -2784,7 +2789,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A177" s="2">
         <v>176</v>
       </c>
@@ -2792,7 +2797,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A178" s="2">
         <v>177</v>
       </c>
@@ -2800,7 +2805,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A179" s="2">
         <v>178</v>
       </c>
@@ -2808,7 +2813,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A180" s="2">
         <v>179</v>
       </c>
@@ -2816,7 +2821,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A181" s="2">
         <v>180</v>
       </c>
@@ -2824,7 +2829,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A182" s="2">
         <v>181</v>
       </c>
@@ -2832,7 +2837,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A183" s="2">
         <v>182</v>
       </c>
@@ -2840,7 +2845,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A184" s="2">
         <v>183</v>
       </c>
@@ -2848,7 +2853,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A185" s="2">
         <v>184</v>
       </c>
@@ -2856,7 +2861,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A186" s="2">
         <v>185</v>
       </c>
@@ -2864,7 +2869,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A187" s="2">
         <v>186</v>
       </c>
@@ -2872,7 +2877,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A188" s="2">
         <v>187</v>
       </c>
@@ -2880,7 +2885,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A189" s="2">
         <v>188</v>
       </c>
@@ -2888,7 +2893,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A190" s="2">
         <v>189</v>
       </c>
@@ -2896,7 +2901,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A191" s="2">
         <v>190</v>
       </c>
@@ -2904,7 +2909,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A192" s="2">
         <v>191</v>
       </c>
@@ -2912,7 +2917,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A193" s="2">
         <v>192</v>
       </c>
@@ -2920,7 +2925,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A194" s="2">
         <v>193</v>
       </c>
@@ -2928,7 +2933,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A195" s="2">
         <v>194</v>
       </c>
@@ -2936,7 +2941,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A196" s="2">
         <v>195</v>
       </c>
@@ -2944,7 +2949,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A197" s="2">
         <v>196</v>
       </c>
@@ -2952,7 +2957,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A198" s="2">
         <v>197</v>
       </c>
@@ -2960,7 +2965,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A199" s="2">
         <v>198</v>
       </c>
@@ -2968,7 +2973,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A200" s="2">
         <v>199</v>
       </c>
@@ -2976,7 +2981,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A201" s="2">
         <v>200</v>
       </c>
@@ -2984,7 +2989,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A202" s="2">
         <v>201</v>
       </c>
@@ -2992,7 +2997,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A203" s="2">
         <v>202</v>
       </c>
@@ -3000,7 +3005,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A204" s="2">
         <v>203</v>
       </c>
@@ -3008,7 +3013,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A205" s="2">
         <v>204</v>
       </c>
@@ -3016,7 +3021,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A206" s="2">
         <v>205</v>
       </c>
@@ -3024,7 +3029,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A207" s="2">
         <v>206</v>
       </c>
@@ -3032,7 +3037,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A208" s="2">
         <v>207</v>
       </c>
@@ -3040,7 +3045,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A209" s="2">
         <v>208</v>
       </c>
@@ -3048,7 +3053,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A210" s="2">
         <v>209</v>
       </c>
@@ -3056,7 +3061,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A211" s="2">
         <v>210</v>
       </c>
@@ -3064,7 +3069,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A212" s="2">
         <v>211</v>
       </c>
@@ -3072,7 +3077,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A213" s="2">
         <v>212</v>
       </c>
@@ -3080,7 +3085,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A214" s="2">
         <v>213</v>
       </c>
@@ -3088,7 +3093,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A215" s="2">
         <v>214</v>
       </c>
@@ -3096,7 +3101,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A216" s="2">
         <v>215</v>
       </c>
@@ -3104,7 +3109,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A217" s="2">
         <v>216</v>
       </c>
@@ -3112,7 +3117,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A218" s="2">
         <v>217</v>
       </c>
@@ -3120,7 +3125,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A219" s="2">
         <v>218</v>
       </c>
@@ -3128,7 +3133,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A220" s="2">
         <v>219</v>
       </c>
@@ -3136,7 +3141,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A221" s="2">
         <v>220</v>
       </c>
@@ -3144,7 +3149,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A222" s="2">
         <v>221</v>
       </c>
@@ -3152,7 +3157,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A223" s="2">
         <v>222</v>
       </c>
@@ -3160,7 +3165,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A224" s="2">
         <v>223</v>
       </c>
@@ -3168,7 +3173,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A225" s="2">
         <v>224</v>
       </c>
@@ -3176,7 +3181,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A226" s="2">
         <v>225</v>
       </c>
@@ -3184,7 +3189,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A227" s="2">
         <v>226</v>
       </c>
@@ -3192,7 +3197,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A228" s="2">
         <v>227</v>
       </c>
@@ -3200,7 +3205,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A229" s="2">
         <v>228</v>
       </c>
@@ -3208,7 +3213,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A230" s="2">
         <v>229</v>
       </c>
@@ -3216,7 +3221,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A231" s="3">
         <v>230</v>
       </c>
@@ -3224,7 +3229,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A232" s="3">
         <v>231</v>
       </c>
@@ -3232,7 +3237,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A233" s="3">
         <v>232</v>
       </c>
@@ -3240,7 +3245,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A234" s="2">
         <v>233</v>
       </c>
@@ -3248,7 +3253,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A235" s="2">
         <v>234</v>
       </c>
@@ -3256,7 +3261,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A236" s="2">
         <v>235</v>
       </c>
@@ -3264,7 +3269,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A237" s="2">
         <v>236</v>
       </c>
@@ -3272,7 +3277,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A238" s="2">
         <v>237</v>
       </c>
@@ -3280,7 +3285,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A239" s="2">
         <v>238</v>
       </c>
@@ -3288,7 +3293,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A240" s="2">
         <v>239</v>
       </c>
@@ -3296,7 +3301,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A241" s="2">
         <v>240</v>
       </c>
@@ -3304,7 +3309,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A242" s="2">
         <v>241</v>
       </c>
@@ -3312,7 +3317,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A243" s="2">
         <v>242</v>
       </c>
@@ -3320,7 +3325,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A244" s="2">
         <v>243</v>
       </c>
@@ -3328,7 +3333,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A245" s="2">
         <v>244</v>
       </c>
@@ -3336,7 +3341,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A246" s="2">
         <v>245</v>
       </c>
@@ -3344,7 +3349,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A247" s="2">
         <v>246</v>
       </c>
@@ -3352,7 +3357,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A248" s="2">
         <v>247</v>
       </c>
@@ -3360,7 +3365,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A249" s="2">
         <v>248</v>
       </c>
@@ -3368,7 +3373,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A250" s="2">
         <v>249</v>
       </c>
@@ -3376,7 +3381,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A251" s="2">
         <v>250</v>
       </c>
@@ -3384,7 +3389,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A252" s="2">
         <v>251</v>
       </c>
@@ -3392,7 +3397,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A253" s="2">
         <v>252</v>
       </c>
@@ -3400,7 +3405,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A254" s="2">
         <v>253</v>
       </c>
@@ -3408,7 +3413,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A255" s="2">
         <v>254</v>
       </c>
@@ -3416,7 +3421,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A256" s="2">
         <v>255</v>
       </c>
@@ -3424,7 +3429,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A257" s="2">
         <v>256</v>
       </c>
@@ -3432,7 +3437,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A258" s="2">
         <v>257</v>
       </c>
@@ -3440,7 +3445,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A259" s="2">
         <v>258</v>
       </c>
@@ -3448,7 +3453,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A260" s="2">
         <v>259</v>
       </c>
@@ -3456,7 +3461,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A261" s="2">
         <v>260</v>
       </c>
@@ -3464,7 +3469,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A262" s="2">
         <v>261</v>
       </c>
@@ -3472,7 +3477,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A263" s="2">
         <v>262</v>
       </c>
@@ -3480,7 +3485,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A264" s="2">
         <v>263</v>
       </c>
@@ -3488,7 +3493,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A265" s="2">
         <v>264</v>
       </c>
@@ -3496,7 +3501,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A266" s="2">
         <v>265</v>
       </c>
@@ -3504,7 +3509,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A267" s="2">
         <v>266</v>
       </c>
@@ -3512,7 +3517,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A268" s="2">
         <v>267</v>
       </c>
@@ -3520,7 +3525,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A269" s="2">
         <v>268</v>
       </c>
@@ -3528,7 +3533,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A270" s="2">
         <v>269</v>
       </c>
@@ -3536,7 +3541,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A271" s="2">
         <v>270</v>
       </c>
@@ -3544,7 +3549,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A272" s="2">
         <v>271</v>
       </c>
@@ -3552,7 +3557,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A273" s="2">
         <v>272</v>
       </c>
@@ -3560,7 +3565,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A274" s="2">
         <v>273</v>
       </c>
@@ -3568,7 +3573,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A275" s="2">
         <v>274</v>
       </c>
@@ -3576,7 +3581,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A276" s="2">
         <v>275</v>
       </c>
@@ -3584,7 +3589,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A277" s="2">
         <v>276</v>
       </c>
@@ -3592,7 +3597,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A278" s="2">
         <v>277</v>
       </c>
@@ -3600,7 +3605,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A279" s="2">
         <v>278</v>
       </c>
@@ -3608,7 +3613,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A280" s="2">
         <v>279</v>
       </c>
@@ -3616,7 +3621,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A281" s="2">
         <v>280</v>
       </c>
@@ -3624,7 +3629,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A282" s="2">
         <v>281</v>
       </c>
@@ -3632,7 +3637,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A283" s="2">
         <v>282</v>
       </c>
@@ -3640,7 +3645,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A284" s="2">
         <v>283</v>
       </c>
@@ -3648,7 +3653,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A285" s="2">
         <v>284</v>
       </c>
@@ -3656,7 +3661,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A286" s="2">
         <v>285</v>
       </c>
@@ -3664,7 +3669,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A287" s="2">
         <v>286</v>
       </c>
@@ -3672,7 +3677,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A288" s="2">
         <v>287</v>
       </c>
@@ -3680,7 +3685,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A289" s="2">
         <v>288</v>
       </c>
@@ -3688,7 +3693,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A290" s="2">
         <v>289</v>
       </c>
@@ -3696,7 +3701,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A291" s="2">
         <v>290</v>
       </c>
@@ -3704,7 +3709,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A292" s="2">
         <v>291</v>
       </c>
@@ -3712,7 +3717,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A293" s="2">
         <v>292</v>
       </c>
@@ -3720,7 +3725,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A294" s="2">
         <v>293</v>
       </c>
@@ -3728,7 +3733,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A295" s="2">
         <v>294</v>
       </c>
@@ -3736,7 +3741,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A296" s="2">
         <v>295</v>
       </c>
@@ -3744,7 +3749,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A297" s="2">
         <v>296</v>
       </c>
@@ -3752,7 +3757,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A298" s="2">
         <v>297</v>
       </c>
@@ -3760,7 +3765,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A299" s="2">
         <v>298</v>
       </c>
@@ -3768,7 +3773,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A300" s="2">
         <v>299</v>
       </c>
@@ -3776,7 +3781,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A301" s="2">
         <v>300</v>
       </c>
@@ -3784,7 +3789,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A302" s="2">
         <v>301</v>
       </c>
@@ -3792,7 +3797,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A303" s="2">
         <v>302</v>
       </c>
@@ -3800,7 +3805,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A304" s="2">
         <v>303</v>
       </c>
@@ -3808,7 +3813,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A305" s="2">
         <v>304</v>
       </c>
@@ -3816,7 +3821,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A306" s="2">
         <v>305</v>
       </c>
@@ -3824,7 +3829,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A307" s="2">
         <v>306</v>
       </c>
@@ -3832,7 +3837,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A308" s="2">
         <v>307</v>
       </c>
@@ -3840,7 +3845,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A309" s="2">
         <v>308</v>
       </c>
@@ -3848,7 +3853,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A310" s="2">
         <v>309</v>
       </c>
@@ -3856,7 +3861,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A311" s="2">
         <v>310</v>
       </c>
@@ -3864,7 +3869,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A312" s="2">
         <v>311</v>
       </c>
@@ -3872,7 +3877,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A313" s="2">
         <v>312</v>
       </c>
@@ -3880,7 +3885,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A314" s="2">
         <v>313</v>
       </c>
@@ -3888,7 +3893,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A315" s="2">
         <v>314</v>
       </c>
@@ -3896,7 +3901,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A316" s="2">
         <v>315</v>
       </c>
@@ -3904,7 +3909,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A317" s="2">
         <v>316</v>
       </c>
@@ -3912,7 +3917,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A318" s="2">
         <v>317</v>
       </c>
@@ -3920,7 +3925,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A319" s="2">
         <v>318</v>
       </c>
@@ -3928,7 +3933,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A320" s="2">
         <v>319</v>
       </c>
@@ -3936,7 +3941,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A321" s="2">
         <v>320</v>
       </c>
@@ -3944,7 +3949,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A322" s="2">
         <v>321</v>
       </c>
@@ -3952,7 +3957,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A323" s="2">
         <v>322</v>
       </c>
@@ -3960,7 +3965,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A324" s="2">
         <v>323</v>
       </c>
@@ -3968,7 +3973,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A325" s="2">
         <v>324</v>
       </c>
@@ -3976,7 +3981,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A326" s="2">
         <v>325</v>
       </c>
@@ -3984,7 +3989,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A327" s="2">
         <v>326</v>
       </c>
@@ -3992,7 +3997,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A328" s="2">
         <v>327</v>
       </c>
@@ -4000,7 +4005,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A329" s="2">
         <v>328</v>
       </c>
@@ -4008,7 +4013,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A330" s="2">
         <v>329</v>
       </c>
@@ -4016,7 +4021,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A331" s="2">
         <v>330</v>
       </c>
@@ -4025,6 +4030,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B331" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a script to scrape property_ke website
</commit_message>
<xml_diff>
--- a/CPI basket.xlsx
+++ b/CPI basket.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive\Desktop\Web Scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47172BBD-1869-446D-BA21-670E6454695A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B300B8-8190-4109-844E-F64040EF488C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basket" sheetId="1" r:id="rId1"/>
@@ -1369,19 +1369,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:B331"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.76953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1389,7 +1390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1397,7 +1398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1405,7 +1406,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1413,7 +1414,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1421,7 +1422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1429,7 +1430,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1437,7 +1438,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1445,7 +1446,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1453,7 +1454,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1461,7 +1462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1469,7 +1470,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1477,7 +1478,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1485,7 +1486,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1493,7 +1494,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1501,7 +1502,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1509,7 +1510,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1517,7 +1518,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1525,7 +1526,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1533,7 +1534,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1541,7 +1542,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1549,7 +1550,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1557,7 +1558,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1565,7 +1566,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1573,7 +1574,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1581,7 +1582,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1589,7 +1590,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1597,7 +1598,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1605,7 +1606,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1613,7 +1614,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1621,7 +1622,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1629,7 +1630,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1637,7 +1638,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1645,7 +1646,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1653,7 +1654,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1661,7 +1662,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1669,7 +1670,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1677,7 +1678,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1685,7 +1686,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1693,7 +1694,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1701,7 +1702,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1709,7 +1710,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1717,7 +1718,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1725,7 +1726,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1733,7 +1734,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1741,7 +1742,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1749,7 +1750,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1757,7 +1758,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1765,7 +1766,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1773,7 +1774,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -1781,7 +1782,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -1789,7 +1790,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -1797,7 +1798,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -1805,7 +1806,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -1813,7 +1814,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -1821,7 +1822,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -1829,7 +1830,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -1837,7 +1838,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -1845,7 +1846,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -1853,7 +1854,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -1861,7 +1862,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -1869,7 +1870,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -1877,7 +1878,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -1885,7 +1886,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -1893,7 +1894,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -1901,7 +1902,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -1909,7 +1910,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -1917,7 +1918,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -1925,7 +1926,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -1933,7 +1934,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -1941,7 +1942,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -1949,7 +1950,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -1957,7 +1958,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -1965,7 +1966,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -1973,7 +1974,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -1981,7 +1982,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -1989,7 +1990,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -1997,7 +1998,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -2005,7 +2006,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -2013,7 +2014,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -2021,7 +2022,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -2029,7 +2030,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -2037,7 +2038,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -2045,7 +2046,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -2053,7 +2054,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -2061,7 +2062,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -2069,7 +2070,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -2077,7 +2078,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -2085,7 +2086,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -2093,7 +2094,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -2101,7 +2102,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -2109,7 +2110,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -2117,7 +2118,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -2125,7 +2126,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -2133,7 +2134,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -2141,7 +2142,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -2149,7 +2150,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="97" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -2157,7 +2158,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="98" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -2165,7 +2166,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="99" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -2173,7 +2174,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="100" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -2181,7 +2182,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="101" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -2189,7 +2190,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="102" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -2197,7 +2198,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="103" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -2205,7 +2206,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="104" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -2213,7 +2214,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="105" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -2221,7 +2222,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="106" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -2229,7 +2230,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="107" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -2237,7 +2238,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="108" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -2245,7 +2246,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="109" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -2253,7 +2254,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="110" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>109</v>
       </c>
@@ -2261,7 +2262,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="111" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -2269,7 +2270,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="112" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -2277,7 +2278,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -2285,7 +2286,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -2293,7 +2294,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -2301,7 +2302,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -2309,7 +2310,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -2317,7 +2318,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -2325,7 +2326,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -2333,7 +2334,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>119</v>
       </c>
@@ -2341,7 +2342,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -2349,7 +2350,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>121</v>
       </c>
@@ -2357,7 +2358,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -2365,7 +2366,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>123</v>
       </c>
@@ -2373,7 +2374,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>124</v>
       </c>
@@ -2381,7 +2382,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>125</v>
       </c>
@@ -2389,7 +2390,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>126</v>
       </c>
@@ -2397,7 +2398,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>127</v>
       </c>
@@ -2405,7 +2406,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>128</v>
       </c>
@@ -2413,7 +2414,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>129</v>
       </c>
@@ -2421,7 +2422,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>130</v>
       </c>
@@ -2429,7 +2430,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>131</v>
       </c>
@@ -2437,7 +2438,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>132</v>
       </c>
@@ -2445,7 +2446,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>133</v>
       </c>
@@ -2453,7 +2454,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>134</v>
       </c>
@@ -2461,7 +2462,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>135</v>
       </c>
@@ -2469,7 +2470,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>136</v>
       </c>
@@ -2477,7 +2478,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>137</v>
       </c>
@@ -2485,7 +2486,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>138</v>
       </c>
@@ -2493,7 +2494,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>139</v>
       </c>
@@ -2501,7 +2502,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>140</v>
       </c>
@@ -2509,7 +2510,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>141</v>
       </c>
@@ -2517,7 +2518,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>142</v>
       </c>
@@ -2525,7 +2526,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>143</v>
       </c>
@@ -2533,7 +2534,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>144</v>
       </c>
@@ -2541,7 +2542,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>145</v>
       </c>
@@ -2549,7 +2550,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>146</v>
       </c>
@@ -2557,7 +2558,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>147</v>
       </c>
@@ -2565,7 +2566,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>148</v>
       </c>
@@ -2573,7 +2574,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>149</v>
       </c>
@@ -2581,7 +2582,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>150</v>
       </c>
@@ -2589,7 +2590,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>151</v>
       </c>
@@ -2597,7 +2598,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>152</v>
       </c>
@@ -2605,7 +2606,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="154" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>153</v>
       </c>
@@ -2613,7 +2614,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>154</v>
       </c>
@@ -2621,7 +2622,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="156" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>155</v>
       </c>
@@ -2629,7 +2630,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="157" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>156</v>
       </c>
@@ -2637,7 +2638,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>157</v>
       </c>
@@ -2645,7 +2646,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="159" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>158</v>
       </c>
@@ -2653,7 +2654,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>159</v>
       </c>
@@ -2661,7 +2662,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>160</v>
       </c>
@@ -2669,7 +2670,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>161</v>
       </c>
@@ -2677,7 +2678,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>162</v>
       </c>
@@ -2685,7 +2686,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>163</v>
       </c>
@@ -2693,7 +2694,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>164</v>
       </c>
@@ -2701,7 +2702,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="166" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>165</v>
       </c>
@@ -2709,7 +2710,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>166</v>
       </c>
@@ -2717,7 +2718,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="168" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>167</v>
       </c>
@@ -2725,7 +2726,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>168</v>
       </c>
@@ -2733,7 +2734,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="170" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>169</v>
       </c>
@@ -2741,7 +2742,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>170</v>
       </c>
@@ -2749,7 +2750,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>171</v>
       </c>
@@ -2757,7 +2758,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>172</v>
       </c>
@@ -2765,7 +2766,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>173</v>
       </c>
@@ -2773,7 +2774,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="175" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>174</v>
       </c>
@@ -2781,7 +2782,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <v>175</v>
       </c>
@@ -2789,7 +2790,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <v>176</v>
       </c>
@@ -2797,7 +2798,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>177</v>
       </c>
@@ -2805,7 +2806,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>178</v>
       </c>
@@ -2813,7 +2814,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>179</v>
       </c>
@@ -2821,7 +2822,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>180</v>
       </c>
@@ -2829,7 +2830,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>181</v>
       </c>
@@ -2837,7 +2838,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>182</v>
       </c>
@@ -2845,7 +2846,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>183</v>
       </c>
@@ -2853,7 +2854,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>184</v>
       </c>
@@ -2861,7 +2862,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>185</v>
       </c>
@@ -2869,7 +2870,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>186</v>
       </c>
@@ -2877,7 +2878,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>187</v>
       </c>
@@ -2885,7 +2886,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>188</v>
       </c>
@@ -2893,7 +2894,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>189</v>
       </c>
@@ -2901,7 +2902,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>190</v>
       </c>
@@ -2909,7 +2910,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>191</v>
       </c>
@@ -2917,7 +2918,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <v>192</v>
       </c>
@@ -2925,7 +2926,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
         <v>193</v>
       </c>
@@ -2933,7 +2934,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <v>194</v>
       </c>
@@ -2941,7 +2942,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <v>195</v>
       </c>
@@ -2949,7 +2950,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
         <v>196</v>
       </c>
@@ -2957,7 +2958,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="198" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <v>197</v>
       </c>
@@ -2965,7 +2966,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <v>198</v>
       </c>
@@ -2973,7 +2974,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
         <v>199</v>
       </c>
@@ -2981,7 +2982,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <v>200</v>
       </c>
@@ -2989,7 +2990,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
         <v>201</v>
       </c>
@@ -2997,7 +2998,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
         <v>202</v>
       </c>
@@ -3005,7 +3006,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
         <v>203</v>
       </c>
@@ -3013,7 +3014,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <v>204</v>
       </c>
@@ -3021,7 +3022,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
         <v>205</v>
       </c>
@@ -3029,7 +3030,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
         <v>206</v>
       </c>
@@ -3037,7 +3038,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
         <v>207</v>
       </c>
@@ -3045,7 +3046,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <v>208</v>
       </c>
@@ -3053,7 +3054,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <v>209</v>
       </c>
@@ -3061,7 +3062,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <v>210</v>
       </c>
@@ -3069,7 +3070,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <v>211</v>
       </c>
@@ -3077,7 +3078,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>212</v>
       </c>
@@ -3085,7 +3086,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>213</v>
       </c>
@@ -3093,7 +3094,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>214</v>
       </c>
@@ -3101,7 +3102,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <v>215</v>
       </c>
@@ -3109,7 +3110,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <v>216</v>
       </c>
@@ -3117,7 +3118,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="218" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <v>217</v>
       </c>
@@ -3125,7 +3126,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>218</v>
       </c>
@@ -3133,7 +3134,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <v>219</v>
       </c>
@@ -3141,7 +3142,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
         <v>220</v>
       </c>
@@ -3149,7 +3150,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <v>221</v>
       </c>
@@ -3157,7 +3158,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>222</v>
       </c>
@@ -3165,7 +3166,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <v>223</v>
       </c>
@@ -3173,7 +3174,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
         <v>224</v>
       </c>
@@ -3181,7 +3182,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
         <v>225</v>
       </c>
@@ -3189,7 +3190,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
         <v>226</v>
       </c>
@@ -3197,7 +3198,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
         <v>227</v>
       </c>
@@ -3205,7 +3206,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
         <v>228</v>
       </c>
@@ -3213,7 +3214,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
         <v>229</v>
       </c>
@@ -3221,7 +3222,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="3">
         <v>230</v>
       </c>
@@ -3229,7 +3230,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="3">
         <v>231</v>
       </c>
@@ -3237,7 +3238,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="3">
         <v>232</v>
       </c>
@@ -3245,7 +3246,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="2">
         <v>233</v>
       </c>
@@ -3253,7 +3254,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="2">
         <v>234</v>
       </c>
@@ -3261,7 +3262,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="2">
         <v>235</v>
       </c>
@@ -3269,7 +3270,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="2">
         <v>236</v>
       </c>
@@ -3277,7 +3278,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="2">
         <v>237</v>
       </c>
@@ -3285,7 +3286,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="2">
         <v>238</v>
       </c>
@@ -3293,7 +3294,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="240" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="2">
         <v>239</v>
       </c>
@@ -3301,7 +3302,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="2">
         <v>240</v>
       </c>
@@ -3309,7 +3310,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="242" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="2">
         <v>241</v>
       </c>
@@ -3317,7 +3318,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="243" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="2">
         <v>242</v>
       </c>
@@ -3325,7 +3326,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="244" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="2">
         <v>243</v>
       </c>
@@ -3333,7 +3334,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="2">
         <v>244</v>
       </c>
@@ -3341,7 +3342,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="246" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="2">
         <v>245</v>
       </c>
@@ -3349,7 +3350,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="2">
         <v>246</v>
       </c>
@@ -3357,7 +3358,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="248" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="2">
         <v>247</v>
       </c>
@@ -3365,7 +3366,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="2">
         <v>248</v>
       </c>
@@ -3373,7 +3374,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="250" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="2">
         <v>249</v>
       </c>
@@ -3381,7 +3382,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="2">
         <v>250</v>
       </c>
@@ -3389,7 +3390,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="252" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="2">
         <v>251</v>
       </c>
@@ -3397,7 +3398,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="253" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="2">
         <v>252</v>
       </c>
@@ -3405,7 +3406,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="254" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="2">
         <v>253</v>
       </c>
@@ -3413,7 +3414,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="255" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="2">
         <v>254</v>
       </c>
@@ -3421,7 +3422,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="256" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="2">
         <v>255</v>
       </c>
@@ -3429,7 +3430,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="257" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="2">
         <v>256</v>
       </c>
@@ -3437,7 +3438,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="258" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="2">
         <v>257</v>
       </c>
@@ -3445,7 +3446,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="259" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="2">
         <v>258</v>
       </c>
@@ -3453,7 +3454,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="260" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="2">
         <v>259</v>
       </c>
@@ -3461,7 +3462,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="261" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="2">
         <v>260</v>
       </c>
@@ -3469,7 +3470,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="262" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="2">
         <v>261</v>
       </c>
@@ -3477,7 +3478,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="263" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="2">
         <v>262</v>
       </c>
@@ -3485,7 +3486,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="264" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="2">
         <v>263</v>
       </c>
@@ -3493,7 +3494,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="265" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="2">
         <v>264</v>
       </c>
@@ -3501,7 +3502,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="266" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="2">
         <v>265</v>
       </c>
@@ -3509,7 +3510,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="267" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="2">
         <v>266</v>
       </c>
@@ -3517,7 +3518,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="268" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="2">
         <v>267</v>
       </c>
@@ -3525,7 +3526,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="269" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="2">
         <v>268</v>
       </c>
@@ -3533,7 +3534,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="270" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="2">
         <v>269</v>
       </c>
@@ -3541,7 +3542,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="271" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="2">
         <v>270</v>
       </c>
@@ -3549,7 +3550,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="272" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="2">
         <v>271</v>
       </c>
@@ -3557,7 +3558,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="273" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="2">
         <v>272</v>
       </c>
@@ -3565,7 +3566,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="274" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="2">
         <v>273</v>
       </c>
@@ -3573,7 +3574,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="275" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="2">
         <v>274</v>
       </c>
@@ -3581,7 +3582,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="276" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="2">
         <v>275</v>
       </c>
@@ -3589,7 +3590,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="277" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="2">
         <v>276</v>
       </c>
@@ -3597,7 +3598,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="278" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="2">
         <v>277</v>
       </c>
@@ -3605,7 +3606,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="279" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="2">
         <v>278</v>
       </c>
@@ -3613,7 +3614,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="280" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="2">
         <v>279</v>
       </c>
@@ -3621,7 +3622,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="281" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="2">
         <v>280</v>
       </c>
@@ -3629,7 +3630,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="282" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="2">
         <v>281</v>
       </c>
@@ -3637,7 +3638,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="283" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="2">
         <v>282</v>
       </c>
@@ -3645,7 +3646,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="284" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="2">
         <v>283</v>
       </c>
@@ -3653,7 +3654,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="285" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="2">
         <v>284</v>
       </c>
@@ -3661,7 +3662,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="286" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="2">
         <v>285</v>
       </c>
@@ -3669,7 +3670,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="287" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="2">
         <v>286</v>
       </c>
@@ -3677,7 +3678,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="288" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="2">
         <v>287</v>
       </c>
@@ -3685,7 +3686,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="289" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="2">
         <v>288</v>
       </c>
@@ -3693,7 +3694,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="290" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="2">
         <v>289</v>
       </c>
@@ -3701,7 +3702,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="291" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="2">
         <v>290</v>
       </c>
@@ -3709,7 +3710,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="292" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="2">
         <v>291</v>
       </c>
@@ -3717,7 +3718,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="293" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="2">
         <v>292</v>
       </c>
@@ -3725,7 +3726,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="294" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="2">
         <v>293</v>
       </c>
@@ -3733,7 +3734,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="295" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="2">
         <v>294</v>
       </c>
@@ -3741,7 +3742,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="296" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" s="2">
         <v>295</v>
       </c>
@@ -3749,7 +3750,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="297" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="2">
         <v>296</v>
       </c>
@@ -3757,7 +3758,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="298" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="2">
         <v>297</v>
       </c>
@@ -3765,7 +3766,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="299" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="2">
         <v>298</v>
       </c>
@@ -3773,7 +3774,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="300" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" s="2">
         <v>299</v>
       </c>
@@ -3781,7 +3782,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="301" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="2">
         <v>300</v>
       </c>
@@ -3789,7 +3790,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="302" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" s="2">
         <v>301</v>
       </c>
@@ -3797,7 +3798,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="303" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="2">
         <v>302</v>
       </c>
@@ -3805,7 +3806,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="304" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="2">
         <v>303</v>
       </c>
@@ -3813,7 +3814,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="305" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" s="2">
         <v>304</v>
       </c>
@@ -3821,7 +3822,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="306" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="2">
         <v>305</v>
       </c>
@@ -3829,7 +3830,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="307" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" s="2">
         <v>306</v>
       </c>
@@ -3837,7 +3838,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="308" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" s="2">
         <v>307</v>
       </c>
@@ -3845,7 +3846,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="309" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="2">
         <v>308</v>
       </c>
@@ -3853,7 +3854,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="310" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="2">
         <v>309</v>
       </c>
@@ -3861,7 +3862,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="311" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="2">
         <v>310</v>
       </c>
@@ -3869,7 +3870,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="312" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="2">
         <v>311</v>
       </c>
@@ -3877,7 +3878,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="313" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="2">
         <v>312</v>
       </c>
@@ -3885,7 +3886,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="314" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" s="2">
         <v>313</v>
       </c>
@@ -3893,7 +3894,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="315" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" s="2">
         <v>314</v>
       </c>
@@ -3901,7 +3902,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="316" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" s="2">
         <v>315</v>
       </c>
@@ -3909,7 +3910,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="317" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" s="2">
         <v>316</v>
       </c>
@@ -3917,7 +3918,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="318" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" s="2">
         <v>317</v>
       </c>
@@ -3925,7 +3926,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="319" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" s="2">
         <v>318</v>
       </c>
@@ -3933,7 +3934,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="320" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" s="2">
         <v>319</v>
       </c>
@@ -3941,7 +3942,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="321" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" s="2">
         <v>320</v>
       </c>
@@ -3949,7 +3950,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="322" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" s="2">
         <v>321</v>
       </c>
@@ -3957,7 +3958,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="323" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" s="2">
         <v>322</v>
       </c>
@@ -3965,7 +3966,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="324" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" s="2">
         <v>323</v>
       </c>
@@ -3973,7 +3974,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="325" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" s="2">
         <v>324</v>
       </c>
@@ -3981,7 +3982,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="326" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" s="2">
         <v>325</v>
       </c>
@@ -3989,7 +3990,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="327" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" s="2">
         <v>326</v>
       </c>
@@ -3997,7 +3998,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="328" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" s="2">
         <v>327</v>
       </c>
@@ -4005,7 +4006,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="329" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" s="2">
         <v>328</v>
       </c>
@@ -4013,7 +4014,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="330" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" s="2">
         <v>329</v>
       </c>
@@ -4021,7 +4022,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="331" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" s="2">
         <v>330</v>
       </c>
@@ -4030,7 +4031,19 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B331" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:B331" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Actual monthly house rent - 1 bedroom"/>
+        <filter val="Actual monthly house rent - 2 bedroom"/>
+        <filter val="Actual monthly house rent - 3 bedroom"/>
+        <filter val="Actual monthly house rent - bed sitter"/>
+        <filter val="Actual monthly house rent - double room"/>
+        <filter val="Actual monthly house rent - single room"/>
+        <filter val="Actual monthly house rent -more than 3 bedroom"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Didsome testing on the Script
</commit_message>
<xml_diff>
--- a/CPI basket.xlsx
+++ b/CPI basket.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive\Desktop\Web Scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B300B8-8190-4109-844E-F64040EF488C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FD9D5D-3CC5-4470-9D2D-D703FF98A9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-270" yWindow="-270" windowWidth="29340" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basket" sheetId="1" r:id="rId1"/>
@@ -1369,20 +1369,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:B331"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1390,7 +1389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1398,7 +1397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1406,7 +1405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1414,7 +1413,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1422,7 +1421,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1430,7 +1429,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1438,7 +1437,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1446,7 +1445,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1454,7 +1453,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1462,7 +1461,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1470,7 +1469,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1478,7 +1477,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1486,7 +1485,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1494,7 +1493,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1502,7 +1501,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1510,7 +1509,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1518,7 +1517,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1526,7 +1525,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1534,7 +1533,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1542,7 +1541,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1550,7 +1549,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1558,7 +1557,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1566,7 +1565,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1574,7 +1573,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1582,7 +1581,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1590,7 +1589,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1598,7 +1597,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1606,7 +1605,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1614,7 +1613,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1622,7 +1621,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1630,7 +1629,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1638,7 +1637,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1646,7 +1645,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1654,7 +1653,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1662,7 +1661,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1670,7 +1669,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1678,7 +1677,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1686,7 +1685,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1694,7 +1693,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1702,7 +1701,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1710,7 +1709,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1718,7 +1717,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1726,7 +1725,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1734,7 +1733,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1742,7 +1741,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1750,7 +1749,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1758,7 +1757,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1766,7 +1765,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1774,7 +1773,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -1782,7 +1781,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -1790,7 +1789,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -1798,7 +1797,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -1806,7 +1805,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -1814,7 +1813,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -1822,7 +1821,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -1830,7 +1829,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -1838,7 +1837,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -1846,7 +1845,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -1854,7 +1853,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -1862,7 +1861,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -1870,7 +1869,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -1878,7 +1877,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -1886,7 +1885,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -1894,7 +1893,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -1902,7 +1901,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -1910,7 +1909,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -1918,7 +1917,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -1926,7 +1925,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -1934,7 +1933,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -1942,7 +1941,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -1950,7 +1949,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -1958,7 +1957,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -1966,7 +1965,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -1974,7 +1973,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -1982,7 +1981,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -1990,7 +1989,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -1998,7 +1997,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -2006,7 +2005,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -2014,7 +2013,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -2022,7 +2021,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -2030,7 +2029,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -2038,7 +2037,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -2046,7 +2045,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -2054,7 +2053,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -2062,7 +2061,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -2070,7 +2069,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -2078,7 +2077,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -2086,7 +2085,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -2094,7 +2093,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -2102,7 +2101,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -2110,7 +2109,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -2118,7 +2117,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -2126,7 +2125,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -2134,7 +2133,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -2142,7 +2141,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -2150,7 +2149,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="97" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -2158,7 +2157,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="98" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -2166,7 +2165,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="99" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -2174,7 +2173,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="100" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -2182,7 +2181,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="101" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -2190,7 +2189,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="102" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -2198,7 +2197,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="103" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -2206,7 +2205,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="104" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -2214,7 +2213,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="105" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -2222,7 +2221,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="106" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -2230,7 +2229,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="107" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -2238,7 +2237,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="108" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -2246,7 +2245,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="109" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -2254,7 +2253,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="110" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A110" s="2">
         <v>109</v>
       </c>
@@ -2262,7 +2261,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="111" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -2270,7 +2269,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="112" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -2278,7 +2277,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -2286,7 +2285,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -2294,7 +2293,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -2302,7 +2301,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -2310,7 +2309,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -2318,7 +2317,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -2326,7 +2325,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -2334,7 +2333,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A120" s="2">
         <v>119</v>
       </c>
@@ -2342,7 +2341,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -2350,7 +2349,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A122" s="2">
         <v>121</v>
       </c>
@@ -2358,7 +2357,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -2366,7 +2365,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A124" s="2">
         <v>123</v>
       </c>
@@ -2374,7 +2373,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A125" s="2">
         <v>124</v>
       </c>
@@ -2382,7 +2381,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A126" s="2">
         <v>125</v>
       </c>
@@ -2390,7 +2389,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A127" s="2">
         <v>126</v>
       </c>
@@ -2398,7 +2397,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A128" s="2">
         <v>127</v>
       </c>
@@ -2406,7 +2405,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A129" s="2">
         <v>128</v>
       </c>
@@ -2414,7 +2413,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A130" s="2">
         <v>129</v>
       </c>
@@ -2422,7 +2421,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A131" s="2">
         <v>130</v>
       </c>
@@ -2430,7 +2429,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A132" s="2">
         <v>131</v>
       </c>
@@ -2438,7 +2437,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A133" s="2">
         <v>132</v>
       </c>
@@ -2446,7 +2445,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A134" s="2">
         <v>133</v>
       </c>
@@ -2454,7 +2453,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A135" s="2">
         <v>134</v>
       </c>
@@ -2462,7 +2461,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A136" s="2">
         <v>135</v>
       </c>
@@ -2470,7 +2469,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A137" s="2">
         <v>136</v>
       </c>
@@ -2478,7 +2477,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A138" s="2">
         <v>137</v>
       </c>
@@ -2486,7 +2485,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A139" s="2">
         <v>138</v>
       </c>
@@ -2494,7 +2493,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A140" s="2">
         <v>139</v>
       </c>
@@ -2502,7 +2501,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A141" s="2">
         <v>140</v>
       </c>
@@ -2510,7 +2509,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A142" s="2">
         <v>141</v>
       </c>
@@ -2518,7 +2517,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A143" s="2">
         <v>142</v>
       </c>
@@ -2526,7 +2525,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A144" s="2">
         <v>143</v>
       </c>
@@ -2534,7 +2533,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A145" s="2">
         <v>144</v>
       </c>
@@ -2542,7 +2541,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A146" s="2">
         <v>145</v>
       </c>
@@ -2550,7 +2549,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A147" s="2">
         <v>146</v>
       </c>
@@ -2558,7 +2557,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A148" s="2">
         <v>147</v>
       </c>
@@ -2566,7 +2565,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A149" s="2">
         <v>148</v>
       </c>
@@ -2574,7 +2573,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A150" s="2">
         <v>149</v>
       </c>
@@ -2582,7 +2581,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A151" s="2">
         <v>150</v>
       </c>
@@ -2590,7 +2589,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A152" s="2">
         <v>151</v>
       </c>
@@ -2598,7 +2597,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A153" s="2">
         <v>152</v>
       </c>
@@ -2606,7 +2605,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="154" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A154" s="2">
         <v>153</v>
       </c>
@@ -2614,7 +2613,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A155" s="2">
         <v>154</v>
       </c>
@@ -2622,7 +2621,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="156" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A156" s="2">
         <v>155</v>
       </c>
@@ -2630,7 +2629,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="157" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A157" s="2">
         <v>156</v>
       </c>
@@ -2638,7 +2637,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A158" s="2">
         <v>157</v>
       </c>
@@ -2646,7 +2645,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="159" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A159" s="2">
         <v>158</v>
       </c>
@@ -2654,7 +2653,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A160" s="2">
         <v>159</v>
       </c>
@@ -2662,7 +2661,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A161" s="2">
         <v>160</v>
       </c>
@@ -2670,7 +2669,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A162" s="2">
         <v>161</v>
       </c>
@@ -2678,7 +2677,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A163" s="2">
         <v>162</v>
       </c>
@@ -2686,7 +2685,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A164" s="2">
         <v>163</v>
       </c>
@@ -2694,7 +2693,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A165" s="2">
         <v>164</v>
       </c>
@@ -2702,7 +2701,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="166" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A166" s="2">
         <v>165</v>
       </c>
@@ -2710,7 +2709,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A167" s="2">
         <v>166</v>
       </c>
@@ -2718,7 +2717,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="168" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A168" s="2">
         <v>167</v>
       </c>
@@ -2726,7 +2725,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A169" s="2">
         <v>168</v>
       </c>
@@ -2734,7 +2733,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="170" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A170" s="2">
         <v>169</v>
       </c>
@@ -2742,7 +2741,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A171" s="2">
         <v>170</v>
       </c>
@@ -2750,7 +2749,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A172" s="2">
         <v>171</v>
       </c>
@@ -2758,7 +2757,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A173" s="2">
         <v>172</v>
       </c>
@@ -2766,7 +2765,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A174" s="2">
         <v>173</v>
       </c>
@@ -2774,7 +2773,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="175" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A175" s="2">
         <v>174</v>
       </c>
@@ -2782,7 +2781,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A176" s="2">
         <v>175</v>
       </c>
@@ -2790,7 +2789,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A177" s="2">
         <v>176</v>
       </c>
@@ -2798,7 +2797,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A178" s="2">
         <v>177</v>
       </c>
@@ -2806,7 +2805,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A179" s="2">
         <v>178</v>
       </c>
@@ -2814,7 +2813,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A180" s="2">
         <v>179</v>
       </c>
@@ -2822,7 +2821,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A181" s="2">
         <v>180</v>
       </c>
@@ -2830,7 +2829,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A182" s="2">
         <v>181</v>
       </c>
@@ -2838,7 +2837,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A183" s="2">
         <v>182</v>
       </c>
@@ -2846,7 +2845,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A184" s="2">
         <v>183</v>
       </c>
@@ -2854,7 +2853,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A185" s="2">
         <v>184</v>
       </c>
@@ -2862,7 +2861,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A186" s="2">
         <v>185</v>
       </c>
@@ -2870,7 +2869,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A187" s="2">
         <v>186</v>
       </c>
@@ -2878,7 +2877,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A188" s="2">
         <v>187</v>
       </c>
@@ -2886,7 +2885,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A189" s="2">
         <v>188</v>
       </c>
@@ -2894,7 +2893,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A190" s="2">
         <v>189</v>
       </c>
@@ -2902,7 +2901,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A191" s="2">
         <v>190</v>
       </c>
@@ -2910,7 +2909,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A192" s="2">
         <v>191</v>
       </c>
@@ -2918,7 +2917,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A193" s="2">
         <v>192</v>
       </c>
@@ -2926,7 +2925,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A194" s="2">
         <v>193</v>
       </c>
@@ -2934,7 +2933,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A195" s="2">
         <v>194</v>
       </c>
@@ -2942,7 +2941,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A196" s="2">
         <v>195</v>
       </c>
@@ -2950,7 +2949,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A197" s="2">
         <v>196</v>
       </c>
@@ -2958,7 +2957,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="198" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A198" s="2">
         <v>197</v>
       </c>
@@ -2966,7 +2965,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A199" s="2">
         <v>198</v>
       </c>
@@ -2974,7 +2973,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A200" s="2">
         <v>199</v>
       </c>
@@ -2982,7 +2981,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A201" s="2">
         <v>200</v>
       </c>
@@ -2990,7 +2989,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A202" s="2">
         <v>201</v>
       </c>
@@ -2998,7 +2997,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A203" s="2">
         <v>202</v>
       </c>
@@ -3006,7 +3005,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A204" s="2">
         <v>203</v>
       </c>
@@ -3014,7 +3013,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A205" s="2">
         <v>204</v>
       </c>
@@ -3022,7 +3021,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A206" s="2">
         <v>205</v>
       </c>
@@ -3030,7 +3029,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A207" s="2">
         <v>206</v>
       </c>
@@ -3038,7 +3037,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A208" s="2">
         <v>207</v>
       </c>
@@ -3046,7 +3045,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A209" s="2">
         <v>208</v>
       </c>
@@ -3054,7 +3053,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A210" s="2">
         <v>209</v>
       </c>
@@ -3062,7 +3061,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A211" s="2">
         <v>210</v>
       </c>
@@ -3070,7 +3069,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A212" s="2">
         <v>211</v>
       </c>
@@ -3078,7 +3077,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A213" s="2">
         <v>212</v>
       </c>
@@ -3086,7 +3085,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A214" s="2">
         <v>213</v>
       </c>
@@ -3094,7 +3093,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A215" s="2">
         <v>214</v>
       </c>
@@ -3102,7 +3101,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A216" s="2">
         <v>215</v>
       </c>
@@ -3110,7 +3109,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A217" s="2">
         <v>216</v>
       </c>
@@ -3118,7 +3117,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="218" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A218" s="2">
         <v>217</v>
       </c>
@@ -3126,7 +3125,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A219" s="2">
         <v>218</v>
       </c>
@@ -3134,7 +3133,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A220" s="2">
         <v>219</v>
       </c>
@@ -3142,7 +3141,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A221" s="2">
         <v>220</v>
       </c>
@@ -3150,7 +3149,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A222" s="2">
         <v>221</v>
       </c>
@@ -3158,7 +3157,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A223" s="2">
         <v>222</v>
       </c>
@@ -3166,7 +3165,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A224" s="2">
         <v>223</v>
       </c>
@@ -3174,7 +3173,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A225" s="2">
         <v>224</v>
       </c>
@@ -3182,7 +3181,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A226" s="2">
         <v>225</v>
       </c>
@@ -3190,7 +3189,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A227" s="2">
         <v>226</v>
       </c>
@@ -3198,7 +3197,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A228" s="2">
         <v>227</v>
       </c>
@@ -3206,7 +3205,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A229" s="2">
         <v>228</v>
       </c>
@@ -3214,7 +3213,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A230" s="2">
         <v>229</v>
       </c>
@@ -3222,7 +3221,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A231" s="3">
         <v>230</v>
       </c>
@@ -3230,7 +3229,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A232" s="3">
         <v>231</v>
       </c>
@@ -3238,7 +3237,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A233" s="3">
         <v>232</v>
       </c>
@@ -3246,7 +3245,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A234" s="2">
         <v>233</v>
       </c>
@@ -3254,7 +3253,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A235" s="2">
         <v>234</v>
       </c>
@@ -3262,7 +3261,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A236" s="2">
         <v>235</v>
       </c>
@@ -3270,7 +3269,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A237" s="2">
         <v>236</v>
       </c>
@@ -3278,7 +3277,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A238" s="2">
         <v>237</v>
       </c>
@@ -3286,7 +3285,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A239" s="2">
         <v>238</v>
       </c>
@@ -3294,7 +3293,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="240" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A240" s="2">
         <v>239</v>
       </c>
@@ -3302,7 +3301,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A241" s="2">
         <v>240</v>
       </c>
@@ -3310,7 +3309,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="242" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A242" s="2">
         <v>241</v>
       </c>
@@ -3318,7 +3317,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="243" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A243" s="2">
         <v>242</v>
       </c>
@@ -3326,7 +3325,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="244" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A244" s="2">
         <v>243</v>
       </c>
@@ -3334,7 +3333,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A245" s="2">
         <v>244</v>
       </c>
@@ -3342,7 +3341,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="246" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A246" s="2">
         <v>245</v>
       </c>
@@ -3350,7 +3349,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A247" s="2">
         <v>246</v>
       </c>
@@ -3358,7 +3357,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="248" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A248" s="2">
         <v>247</v>
       </c>
@@ -3366,7 +3365,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A249" s="2">
         <v>248</v>
       </c>
@@ -3374,7 +3373,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="250" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A250" s="2">
         <v>249</v>
       </c>
@@ -3382,7 +3381,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A251" s="2">
         <v>250</v>
       </c>
@@ -3390,7 +3389,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="252" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A252" s="2">
         <v>251</v>
       </c>
@@ -3398,7 +3397,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="253" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A253" s="2">
         <v>252</v>
       </c>
@@ -3406,7 +3405,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="254" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A254" s="2">
         <v>253</v>
       </c>
@@ -3414,7 +3413,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="255" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A255" s="2">
         <v>254</v>
       </c>
@@ -3422,7 +3421,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="256" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A256" s="2">
         <v>255</v>
       </c>
@@ -3430,7 +3429,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="257" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A257" s="2">
         <v>256</v>
       </c>
@@ -3438,7 +3437,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="258" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A258" s="2">
         <v>257</v>
       </c>
@@ -3446,7 +3445,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="259" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A259" s="2">
         <v>258</v>
       </c>
@@ -3454,7 +3453,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="260" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A260" s="2">
         <v>259</v>
       </c>
@@ -3462,7 +3461,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="261" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A261" s="2">
         <v>260</v>
       </c>
@@ -3470,7 +3469,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="262" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A262" s="2">
         <v>261</v>
       </c>
@@ -3478,7 +3477,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="263" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A263" s="2">
         <v>262</v>
       </c>
@@ -3486,7 +3485,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="264" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A264" s="2">
         <v>263</v>
       </c>
@@ -3494,7 +3493,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="265" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A265" s="2">
         <v>264</v>
       </c>
@@ -3502,7 +3501,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="266" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A266" s="2">
         <v>265</v>
       </c>
@@ -3510,7 +3509,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="267" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A267" s="2">
         <v>266</v>
       </c>
@@ -3518,7 +3517,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="268" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A268" s="2">
         <v>267</v>
       </c>
@@ -3526,7 +3525,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="269" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A269" s="2">
         <v>268</v>
       </c>
@@ -3534,7 +3533,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="270" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A270" s="2">
         <v>269</v>
       </c>
@@ -3542,7 +3541,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="271" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A271" s="2">
         <v>270</v>
       </c>
@@ -3550,7 +3549,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="272" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A272" s="2">
         <v>271</v>
       </c>
@@ -3558,7 +3557,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="273" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A273" s="2">
         <v>272</v>
       </c>
@@ -3566,7 +3565,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="274" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A274" s="2">
         <v>273</v>
       </c>
@@ -3574,7 +3573,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="275" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A275" s="2">
         <v>274</v>
       </c>
@@ -3582,7 +3581,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="276" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A276" s="2">
         <v>275</v>
       </c>
@@ -3590,7 +3589,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="277" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A277" s="2">
         <v>276</v>
       </c>
@@ -3598,7 +3597,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="278" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A278" s="2">
         <v>277</v>
       </c>
@@ -3606,7 +3605,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="279" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A279" s="2">
         <v>278</v>
       </c>
@@ -3614,7 +3613,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="280" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A280" s="2">
         <v>279</v>
       </c>
@@ -3622,7 +3621,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="281" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A281" s="2">
         <v>280</v>
       </c>
@@ -3630,7 +3629,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="282" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A282" s="2">
         <v>281</v>
       </c>
@@ -3638,7 +3637,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="283" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A283" s="2">
         <v>282</v>
       </c>
@@ -3646,7 +3645,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="284" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A284" s="2">
         <v>283</v>
       </c>
@@ -3654,7 +3653,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="285" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A285" s="2">
         <v>284</v>
       </c>
@@ -3662,7 +3661,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="286" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A286" s="2">
         <v>285</v>
       </c>
@@ -3670,7 +3669,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="287" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A287" s="2">
         <v>286</v>
       </c>
@@ -3678,7 +3677,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="288" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A288" s="2">
         <v>287</v>
       </c>
@@ -3686,7 +3685,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="289" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A289" s="2">
         <v>288</v>
       </c>
@@ -3694,7 +3693,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="290" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A290" s="2">
         <v>289</v>
       </c>
@@ -3702,7 +3701,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="291" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A291" s="2">
         <v>290</v>
       </c>
@@ -3710,7 +3709,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="292" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A292" s="2">
         <v>291</v>
       </c>
@@ -3718,7 +3717,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="293" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A293" s="2">
         <v>292</v>
       </c>
@@ -3726,7 +3725,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="294" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A294" s="2">
         <v>293</v>
       </c>
@@ -3734,7 +3733,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="295" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A295" s="2">
         <v>294</v>
       </c>
@@ -3742,7 +3741,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="296" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A296" s="2">
         <v>295</v>
       </c>
@@ -3750,7 +3749,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="297" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A297" s="2">
         <v>296</v>
       </c>
@@ -3758,7 +3757,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="298" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A298" s="2">
         <v>297</v>
       </c>
@@ -3766,7 +3765,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="299" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A299" s="2">
         <v>298</v>
       </c>
@@ -3774,7 +3773,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="300" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A300" s="2">
         <v>299</v>
       </c>
@@ -3782,7 +3781,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="301" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A301" s="2">
         <v>300</v>
       </c>
@@ -3790,7 +3789,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="302" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A302" s="2">
         <v>301</v>
       </c>
@@ -3798,7 +3797,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="303" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A303" s="2">
         <v>302</v>
       </c>
@@ -3806,7 +3805,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="304" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A304" s="2">
         <v>303</v>
       </c>
@@ -3814,7 +3813,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="305" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A305" s="2">
         <v>304</v>
       </c>
@@ -3822,7 +3821,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="306" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A306" s="2">
         <v>305</v>
       </c>
@@ -3830,7 +3829,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="307" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A307" s="2">
         <v>306</v>
       </c>
@@ -3838,7 +3837,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="308" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A308" s="2">
         <v>307</v>
       </c>
@@ -3846,7 +3845,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="309" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A309" s="2">
         <v>308</v>
       </c>
@@ -3854,7 +3853,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="310" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A310" s="2">
         <v>309</v>
       </c>
@@ -3862,7 +3861,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="311" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A311" s="2">
         <v>310</v>
       </c>
@@ -3870,7 +3869,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="312" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A312" s="2">
         <v>311</v>
       </c>
@@ -3878,7 +3877,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="313" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A313" s="2">
         <v>312</v>
       </c>
@@ -3886,7 +3885,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="314" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A314" s="2">
         <v>313</v>
       </c>
@@ -3894,7 +3893,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="315" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A315" s="2">
         <v>314</v>
       </c>
@@ -3902,7 +3901,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="316" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A316" s="2">
         <v>315</v>
       </c>
@@ -3910,7 +3909,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="317" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A317" s="2">
         <v>316</v>
       </c>
@@ -3918,7 +3917,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="318" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A318" s="2">
         <v>317</v>
       </c>
@@ -3926,7 +3925,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="319" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A319" s="2">
         <v>318</v>
       </c>
@@ -3934,7 +3933,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="320" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A320" s="2">
         <v>319</v>
       </c>
@@ -3942,7 +3941,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="321" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A321" s="2">
         <v>320</v>
       </c>
@@ -3950,7 +3949,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="322" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A322" s="2">
         <v>321</v>
       </c>
@@ -3958,7 +3957,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="323" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A323" s="2">
         <v>322</v>
       </c>
@@ -3966,7 +3965,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="324" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A324" s="2">
         <v>323</v>
       </c>
@@ -3974,7 +3973,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="325" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A325" s="2">
         <v>324</v>
       </c>
@@ -3982,7 +3981,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="326" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A326" s="2">
         <v>325</v>
       </c>
@@ -3990,7 +3989,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="327" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A327" s="2">
         <v>326</v>
       </c>
@@ -3998,7 +3997,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="328" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A328" s="2">
         <v>327</v>
       </c>
@@ -4006,7 +4005,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="329" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A329" s="2">
         <v>328</v>
       </c>
@@ -4014,7 +4013,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="330" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A330" s="2">
         <v>329</v>
       </c>
@@ -4022,7 +4021,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="331" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A331" s="2">
         <v>330</v>
       </c>
@@ -4031,19 +4030,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B331" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Actual monthly house rent - 1 bedroom"/>
-        <filter val="Actual monthly house rent - 2 bedroom"/>
-        <filter val="Actual monthly house rent - 3 bedroom"/>
-        <filter val="Actual monthly house rent - bed sitter"/>
-        <filter val="Actual monthly house rent - double room"/>
-        <filter val="Actual monthly house rent - single room"/>
-        <filter val="Actual monthly house rent -more than 3 bedroom"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:B331" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>